<commit_message>
Added test - checked incorrect emails
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">automationtesting65@gmail.com</t>
   </si>
@@ -29,6 +29,9 @@
     <t xml:space="preserve">automationtesting65@o2.pl</t>
   </si>
   <si>
+    <t xml:space="preserve">automationtesting@onet.pl</t>
+  </si>
+  <si>
     <t xml:space="preserve">automationtesting65gmail.com </t>
   </si>
   <si>
@@ -44,13 +47,31 @@
     <t xml:space="preserve">automationtesting65@@gmail.com </t>
   </si>
   <si>
-    <t xml:space="preserve">automationtesting65@o2.hh</t>
-  </si>
-  <si>
     <t xml:space="preserve">automationtesting65@ll .pl</t>
   </si>
   <si>
     <t xml:space="preserve">Automationtes ting65@ll .pl</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">automationtesting6@onet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">..pl</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -60,7 +81,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -91,6 +112,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,12 +163,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -165,7 +197,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -187,7 +219,15 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="automationtesting@onet.pl"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -206,7 +246,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -216,46 +256,49 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
+      <c r="A1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
+      <c r="A4" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
+      <c r="A5" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>7</v>
+      <c r="A6" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
+      <c r="A8" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" display="automationtesting6@onet"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added items to properties files, created dataProvider for two-columns sheet, added elements to LoginAndCreateAnAccountPage
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="emailCorrect" sheetId="1" state="visible" r:id="rId2"/>
@@ -55,25 +55,7 @@
     <t xml:space="preserve">Automationtes ting65@ll .pl</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">automationtesting6@onet</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">..pl</t>
-    </r>
+    <t xml:space="preserve">automationtesting6@onet..pl</t>
   </si>
   <si>
     <t xml:space="preserve">jan@o2.pl</t>
@@ -343,7 +325,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -389,7 +371,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" display="automationtesting6@onet"/>
+    <hyperlink ref="A8" r:id="rId1" display="automationtesting6@onet..pl"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -408,14 +390,14 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1" style="4" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="1" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,7 +426,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added DataProvider for registration form and filled exec with correct registration data
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="emailCorrect" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="emailIncorrect" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="existingAccount" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="notExistingAccount" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="createAccountFormAllDataRequired" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t xml:space="preserve">automationtesting65@gmail.com</t>
   </si>
@@ -71,6 +72,48 @@
   </si>
   <si>
     <t xml:space="preserve">jan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kowalski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haslo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is my registration data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haslo11A_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haslo**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 1</t>
   </si>
 </sst>
 </file>
@@ -325,7 +368,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -390,7 +433,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -481,4 +524,120 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>88222</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>258147</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>852369874</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>99877</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>258147</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>852369874</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added methods to LoginAndCreateAnAccountPage, test for filling registration form and new elements in properties file
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -13,6 +13,7 @@
     <sheet name="existingAccount" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="notExistingAccount" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="createAccountFormAllDataRequired" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t xml:space="preserve">automationtesting65@gmail.com</t>
   </si>
@@ -80,7 +81,7 @@
     <t xml:space="preserve">Kowalski</t>
   </si>
   <si>
-    <t xml:space="preserve">Haslo</t>
+    <t xml:space="preserve">Password</t>
   </si>
   <si>
     <t xml:space="preserve">Company</t>
@@ -114,6 +115,9 @@
   </si>
   <si>
     <t xml:space="preserve">Company 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address </t>
   </si>
 </sst>
 </file>
@@ -317,7 +321,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -363,7 +367,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A2:K3 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -434,7 +438,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="A2:K3 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -470,7 +474,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="A2:K3 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -533,8 +537,8 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -543,7 +547,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -619,7 +623,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>22</v>
@@ -628,6 +632,79 @@
         <v>1234</v>
       </c>
       <c r="K3" s="0" t="n">
+        <v>852369874</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="A2:K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>99877</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>258147</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="K2" s="0" t="n">
         <v>852369874</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code refactoring. Only one DataProvider
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t xml:space="preserve">automationtesting65@gmail.com</t>
   </si>
@@ -75,49 +75,112 @@
     <t xml:space="preserve">jan</t>
   </si>
   <si>
+    <t xml:space="preserve">Firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address line 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address alias</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jan</t>
   </si>
   <si>
     <t xml:space="preserve">Kowalski</t>
   </si>
   <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
+    <t xml:space="preserve">Password1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lisia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrocław</t>
   </si>
   <si>
     <t xml:space="preserve">This is my registration data</t>
   </si>
   <si>
-    <t xml:space="preserve">My address</t>
+    <t xml:space="preserve">jk@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haslo11A_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prosta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warszawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grażyna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiśniewska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haslo**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Słoneczna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zielona góra</t>
   </si>
   <si>
     <t xml:space="preserve">Jan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haslo11A_*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Company Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haslo**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Company 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address </t>
   </si>
 </sst>
 </file>
@@ -321,7 +384,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A2:K3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -367,7 +430,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A2:K3 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -438,7 +501,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="A2:K3 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -474,7 +537,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="A2:K3 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -535,10 +598,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:K3"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -548,7 +611,9 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,69 +638,122 @@
       <c r="G1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="0" t="n">
-        <v>88222</v>
+      <c r="H1" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>258147</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>852369874</v>
+        <v>24</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>99877</v>
+        <v>88222</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>258147</v>
       </c>
+      <c r="K2" s="0" t="n">
+        <v>852369823</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>1234</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>852369874</v>
+        <v>99877</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>258147</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>12234</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>123123123</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" display="jk@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -654,7 +772,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="A2:K3"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -664,16 +782,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>99877</v>
@@ -684,19 +802,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Added extentReport and ITestListener, added mehtod to test correct data to log in, remove unused code
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="emailCorrect" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="emailIncorrect" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="existingAccount" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="notExistingAccount" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="createAccountFormAllDataRequired" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="existingEmail" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="existingAccount" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="notExistingAccount" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="createAccountFormAllDataRequired" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
   <si>
     <t xml:space="preserve">automationtesting65@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">automationtesting65@o2.pl</t>
+    <t xml:space="preserve">Automationtesting65@o2.pl</t>
   </si>
   <si>
     <t xml:space="preserve">automationtesting@onet.pl</t>
@@ -54,7 +57,7 @@
     <t xml:space="preserve">automationtesting65@ll .pl</t>
   </si>
   <si>
-    <t xml:space="preserve">Automationtes ting65@ll .pl</t>
+    <t xml:space="preserve">Automationtes ting65@ll.pl</t>
   </si>
   <si>
     <t xml:space="preserve">automationtesting6@onet..pl</t>
@@ -63,6 +66,9 @@
     <t xml:space="preserve">jan@o2.pl</t>
   </si>
   <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
     <t xml:space="preserve">haslo</t>
   </si>
   <si>
@@ -81,9 +87,6 @@
     <t xml:space="preserve">Lastname</t>
   </si>
   <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
     <t xml:space="preserve">Company</t>
   </si>
   <si>
@@ -126,9 +129,6 @@
     <t xml:space="preserve">Lisia</t>
   </si>
   <si>
-    <t xml:space="preserve">3/1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wrocław</t>
   </si>
   <si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t xml:space="preserve">Zielona góra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jan </t>
   </si>
 </sst>
 </file>
@@ -190,7 +187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -236,6 +233,13 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF4D4D4D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -279,7 +283,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -296,11 +300,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,7 +369,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF4D4D4D"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -381,7 +389,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -398,19 +406,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="automationtesting@onet.pl"/>
+    <hyperlink ref="A4" r:id="rId1" display="automationtesting@onet.pl"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -427,7 +440,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
@@ -441,7 +454,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,7 +478,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -475,13 +488,20 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" display="automationtesting6@onet..pl"/>
+    <hyperlink ref="A7" r:id="rId1" display="automationtesting65@ll .pl"/>
+    <hyperlink ref="A8" r:id="rId2" display="Automationtes ting65@ll.pl"/>
+    <hyperlink ref="A9" r:id="rId3" display="automationtesting6@onet..pl"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -498,23 +518,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="1" style="4" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -534,55 +555,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="1" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="jann@o2.pl"/>
-    <hyperlink ref="A3" r:id="rId2" display="jan@o2.pl"/>
-    <hyperlink ref="A4" r:id="rId3" display="jann@o2.pl"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -598,161 +599,62 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>88222</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>258147</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>852369823</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>99877</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>258147</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>44</v>
+      <c r="A4" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>12234</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>123123123</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" display="jk@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="jann@o2.pl"/>
+    <hyperlink ref="A4" r:id="rId2" display="jan@o2.pl"/>
+    <hyperlink ref="A5" r:id="rId3" display="jann@o2.pl"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -769,64 +671,162 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>99877</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>258147</v>
+        <v>20</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>88222</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>258147</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>852369823</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>99877</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>258147</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>1234</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>852369874</v>
+      <c r="E4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>12234</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>123123123</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" display="jk@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>